<commit_message>
update campground visitation data
</commit_message>
<xml_diff>
--- a/TravelDemandModel/2022/data/raw_data/Campground_Visitation_JS_v2.xlsx
+++ b/TravelDemandModel/2022/data/raw_data/Campground_Visitation_JS_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Research and Analysis\Transportation\Travel_Demand_Model\2023 Update\Input Data\Campgrounds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbindl\Documents\GitHub\Transportation\TravelDemandModel\2022\data\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CC2D7207-F545-4DE6-A1BF-F17275F1C159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92742396-988E-4095-9F1A-A2B55F72C481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="972" windowWidth="21600" windowHeight="11388" xr2:uid="{E083D92C-E3E3-4436-8D22-C057CD5AC31C}"/>
+    <workbookView xWindow="720" yWindow="2304" windowWidth="22320" windowHeight="9960" xr2:uid="{E083D92C-E3E3-4436-8D22-C057CD5AC31C}"/>
   </bookViews>
   <sheets>
     <sheet name="Campground_Visitation_JS" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="49">
   <si>
     <t>Campground</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>Closed in 2022</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -1024,19 +1027,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFBBFEC3-0AFD-4775-B170-26D5EFFBC22D}">
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1067,8 +1070,11 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1103,7 +1109,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1138,7 +1144,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1173,7 +1179,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1208,7 +1214,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1240,7 +1246,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1266,7 +1272,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1298,7 +1304,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1379,7 +1385,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -1411,7 +1417,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1440,7 +1446,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1472,7 +1478,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1533,7 +1539,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1565,7 +1571,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1594,7 +1600,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1620,7 +1626,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -1646,7 +1652,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1672,7 +1678,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1695,7 +1701,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -1718,7 +1724,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -1741,7 +1747,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -1764,7 +1770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1787,7 +1793,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1810,7 +1816,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -1833,7 +1839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1856,7 +1862,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1902,7 +1908,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -1925,7 +1931,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -1948,7 +1954,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1971,7 +1977,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -1994,7 +2000,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -2017,7 +2023,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -2040,7 +2046,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -2063,7 +2069,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>

</xml_diff>